<commit_message>
further performance optimization on Lang.fieldsOf by fine tune cache key generation
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t xml:space="preserve">Test Environment</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t xml:space="preserve">Commons PropertyUtils</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HuTool</t>
   </si>
   <si>
     <t xml:space="preserve">EasyMapper</t>
@@ -102,11 +105,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -125,11 +129,19 @@
     </font>
     <font>
       <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -326,6 +338,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -335,25 +348,28 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$2:$A$7</c:f>
+              <c:f>Data!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Commons PropertyUtils</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>HuTool</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>EasyMapper</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Java Clone</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Commons BeanUtils</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>OSGL</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>ModelMapper</c:v>
                 </c:pt>
               </c:strCache>
@@ -361,27 +377,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$G$2:$G$7</c:f>
+              <c:f>Data!$G$2:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2724</c:v>
+                  <c:v>2720</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3724</c:v>
+                  <c:v>1150</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1004</c:v>
+                  <c:v>3130</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7346</c:v>
+                  <c:v>942</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3772</c:v>
+                  <c:v>6600</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5746</c:v>
+                  <c:v>1826</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4078</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -389,11 +408,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="5399891"/>
-        <c:axId val="49291107"/>
+        <c:axId val="70444348"/>
+        <c:axId val="65953109"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="5399891"/>
+        <c:axId val="70444348"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -428,14 +447,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49291107"/>
+        <c:crossAx val="65953109"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49291107"/>
+        <c:axId val="65953109"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -488,7 +507,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -517,7 +536,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5399891"/>
+        <c:crossAx val="70444348"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -598,7 +617,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$G$22</c:f>
+              <c:f>Data!$G$23:$G$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -617,6 +636,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -626,7 +646,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$23:$A$25</c:f>
+              <c:f>Data!$A$24:$A$26</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -643,7 +663,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$G$23:$G$25</c:f>
+              <c:f>Data!$G$24:$G$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -662,11 +682,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="98968415"/>
-        <c:axId val="1602115"/>
+        <c:axId val="79508826"/>
+        <c:axId val="47371102"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="98968415"/>
+        <c:axId val="79508826"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -701,14 +721,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1602115"/>
+        <c:crossAx val="47371102"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1602115"/>
+        <c:axId val="47371102"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -761,7 +781,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -790,7 +810,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98968415"/>
+        <c:crossAx val="79508826"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -822,15 +842,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>754920</xdr:colOff>
+      <xdr:colOff>755280</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>9000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>12240</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>683280</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -838,8 +858,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7087680" y="9000"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="7266960" y="9000"/>
+        <a:ext cx="7449120" cy="3402000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -852,15 +872,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>772200</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:colOff>772560</xdr:colOff>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>27000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>29520</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>15480</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>15120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -868,8 +888,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7104960" y="3440520"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="7284240" y="3603240"/>
+        <a:ext cx="5942160" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -895,7 +915,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -948,16 +968,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P25" activeCellId="0" sqref="P25"/>
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6377551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.8418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -988,23 +1008,23 @@
         <v>15</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>3600</v>
+        <v>2450</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>2430</v>
+        <v>3720</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>2700</v>
+        <v>2600</v>
       </c>
       <c r="E2" s="0" t="n">
+        <v>2360</v>
+      </c>
+      <c r="F2" s="0" t="n">
         <v>2470</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>2420</v>
       </c>
       <c r="G2" s="0" t="n">
         <f aca="false">SUM(B2:F2)/5</f>
-        <v>2724</v>
+        <v>2720</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1012,23 +1032,23 @@
         <v>16</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>3970</v>
+        <v>1160</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>3220</v>
+        <v>1500</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>4000</v>
+        <v>1070</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>3520</v>
+        <v>1010</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>3910</v>
+        <v>1010</v>
       </c>
       <c r="G3" s="0" t="n">
         <f aca="false">SUM(B3:F3)/5</f>
-        <v>3724</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1036,23 +1056,23 @@
         <v>17</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>1000</v>
+        <v>3770</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>1000</v>
+        <v>3820</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>970</v>
+        <v>3040</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>1020</v>
+        <v>2530</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>1030</v>
+        <v>2490</v>
       </c>
       <c r="G4" s="0" t="n">
         <f aca="false">SUM(B4:F4)/5</f>
-        <v>1004</v>
+        <v>3130</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1060,23 +1080,23 @@
         <v>18</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>7280</v>
+        <v>1010</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>7180</v>
+        <v>1000</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>7450</v>
+        <v>1090</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>7440</v>
+        <v>690</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>7380</v>
+        <v>920</v>
       </c>
       <c r="G5" s="0" t="n">
         <f aca="false">SUM(B5:F5)/5</f>
-        <v>7346</v>
+        <v>942</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1084,23 +1104,23 @@
         <v>19</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>3840</v>
+        <v>6760</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>3810</v>
+        <v>6780</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>3900</v>
+        <v>6880</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>3790</v>
+        <v>5880</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>3520</v>
+        <v>6700</v>
       </c>
       <c r="G6" s="0" t="n">
         <f aca="false">SUM(B6:F6)/5</f>
-        <v>3772</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1108,94 +1128,94 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>6380</v>
+        <v>1870</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>8740</v>
+        <v>1810</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>4350</v>
+        <v>1820</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>4500</v>
+        <v>1830</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>4760</v>
+        <v>1800</v>
       </c>
       <c r="G7" s="0" t="n">
         <f aca="false">SUM(B7:F7)/5</f>
-        <v>5746</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>14</v>
+      <c r="B8" s="0" t="n">
+        <v>4120</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>4080</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>4100</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>4020</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>4070</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <f aca="false">SUM(B8:F8)/5</f>
+        <v>4078</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="0" t="n">
-        <v>4950</v>
-      </c>
-      <c r="C23" s="0" t="n">
-        <v>3080</v>
-      </c>
-      <c r="D23" s="0" t="n">
-        <v>4550</v>
-      </c>
-      <c r="E23" s="0" t="n">
-        <v>3740</v>
-      </c>
-      <c r="F23" s="0" t="n">
-        <v>3970</v>
-      </c>
-      <c r="G23" s="0" t="n">
-        <f aca="false">SUM(B23:F23)/5</f>
-        <v>4058</v>
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>15200</v>
+        <v>4950</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>11840</v>
+        <v>3080</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>12690</v>
+        <v>4550</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>12000</v>
+        <v>3740</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>11950</v>
+        <v>3970</v>
       </c>
       <c r="G24" s="0" t="n">
         <f aca="false">SUM(B24:F24)/5</f>
-        <v>12736</v>
+        <v>4058</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1203,29 +1223,53 @@
         <v>23</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>2230</v>
+        <v>15200</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>2080</v>
+        <v>11840</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>2210</v>
+        <v>12690</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>2080</v>
+        <v>12000</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>2160</v>
+        <v>11950</v>
       </c>
       <c r="G25" s="0" t="n">
         <f aca="false">SUM(B25:F25)/5</f>
+        <v>12736</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>2230</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>2080</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>2210</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>2080</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>2160</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <f aca="false">SUM(B26:F26)/5</f>
         <v>2152</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
optimize deep copy performance; new benchmark result report; documentation on copy/mapping
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -5,11 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Data" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="shallow copy" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="deep copy" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="clone" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t xml:space="preserve">Test Environment</t>
   </si>
@@ -47,9 +49,6 @@
     <t xml:space="preserve">LinuxMint 18.3</t>
   </si>
   <si>
-    <t xml:space="preserve">Shallow Copy</t>
-  </si>
-  <si>
     <t xml:space="preserve">R1</t>
   </si>
   <si>
@@ -68,6 +67,9 @@
     <t xml:space="preserve">AVG</t>
   </si>
   <si>
+    <t xml:space="preserve">Ops/ms</t>
+  </si>
+  <si>
     <t xml:space="preserve">Commons PropertyUtils</t>
   </si>
   <si>
@@ -89,23 +91,24 @@
     <t xml:space="preserve">ModelMapper</t>
   </si>
   <si>
-    <t xml:space="preserve">Deep Copy</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dozer</t>
   </si>
   <si>
     <t xml:space="preserve">Orika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commons SerializationUtils</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -129,20 +132,28 @@
     </font>
     <font>
       <sz val="13"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="9"/>
-      <color rgb="FF000000"/>
+      <name val="Noto Sans CJK SC Regular"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -188,8 +199,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -207,7 +222,7 @@
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF00CC33"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -240,22 +255,22 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF83CAFF"/>
+      <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF3399FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF579D1C"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF314004"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
@@ -265,7 +280,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -301,7 +316,7 @@
                 </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Shallow Copy Benchmark</a:t>
+              <a:t>Shallow Copy</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -310,6 +325,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.128575598365441"/>
+          <c:y val="0.202568851666935"/>
+          <c:w val="0.745378478303172"/>
+          <c:h val="0.535271380254469"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -319,18 +345,18 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$G$1</c:f>
+              <c:f>'shallow copy'!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AVG</c:v>
+                  <c:v>Ops/ms</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="83caff"/>
+              <a:srgbClr val="314004"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -338,9 +364,32 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:dLblPos val="outEnd"/>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
             <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
+            <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
@@ -348,7 +397,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$2:$A$8</c:f>
+              <c:f>'shallow copy'!$A$2:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -377,30 +426,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$G$2:$G$8</c:f>
+              <c:f>'shallow copy'!$H$2:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2720</c:v>
+                  <c:v>367.647058823529</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1150</c:v>
+                  <c:v>869.565217391304</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3130</c:v>
+                  <c:v>319.488817891374</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>942</c:v>
+                  <c:v>1061.57112526539</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6600</c:v>
+                  <c:v>151.515151515152</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1826</c:v>
+                  <c:v>547.645125958379</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4078</c:v>
+                  <c:v>245.218244237371</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -408,11 +457,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="70444348"/>
-        <c:axId val="65953109"/>
+        <c:axId val="65319659"/>
+        <c:axId val="23571411"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="70444348"/>
+        <c:axId val="65319659"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -433,7 +482,7 @@
           <a:bodyPr/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -442,19 +491,19 @@
                     <a:srgbClr val="ffffff"/>
                   </a:solidFill>
                 </a:uFill>
-                <a:latin typeface="Arial"/>
+                <a:latin typeface="Noto Sans CJK SC Regular"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65953109"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="23571411"/>
+        <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65953109"/>
+        <c:axId val="23571411"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -500,14 +549,14 @@
                     </a:uFill>
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>ms</a:t>
+                  <a:t>Ops</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -536,7 +585,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70444348"/>
+        <c:crossAx val="65319659"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -549,6 +598,16 @@
         </a:ln>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
@@ -563,7 +622,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -599,7 +658,7 @@
                 </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Deep Copy Benchmark</a:t>
+              <a:t>Deep copy</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -617,18 +676,18 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$G$23:$G$23</c:f>
+              <c:f>'deep copy'!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AVG</c:v>
+                  <c:v>Ops/ms</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="83caff"/>
+              <a:srgbClr val="314004"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -636,9 +695,24 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:dLblPos val="outEnd"/>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
             <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
+            <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
@@ -646,7 +720,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$24:$A$26</c:f>
+              <c:f>'deep copy'!$A$2:$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -663,18 +737,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$G$24:$G$26</c:f>
+              <c:f>'deep copy'!$H$2:$H$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4058</c:v>
+                  <c:v>177.683013503909</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12736</c:v>
+                  <c:v>18.2468432961098</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2152</c:v>
+                  <c:v>310.173697270471</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -682,11 +756,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="79508826"/>
-        <c:axId val="47371102"/>
+        <c:axId val="88096783"/>
+        <c:axId val="6453173"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="79508826"/>
+        <c:axId val="88096783"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -716,19 +790,19 @@
                     <a:srgbClr val="ffffff"/>
                   </a:solidFill>
                 </a:uFill>
-                <a:latin typeface="Arial"/>
+                <a:latin typeface="Noto Sans CJK SC Regular"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47371102"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="6453173"/>
+        <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47371102"/>
+        <c:axId val="6453173"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -774,14 +848,14 @@
                     </a:uFill>
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>ms</a:t>
+                  <a:t>Ops</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -810,7 +884,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79508826"/>
+        <c:crossAx val="88096783"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -823,6 +897,301 @@
         </a:ln>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Clone - Deep copy</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>clone!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ops/ms</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="314004"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>clone!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Commons SerializationUtils</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OSGL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>clone!$H$2:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>46.7901927755942</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>108.178277801817</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="12706079"/>
+        <c:axId val="21330574"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="12706079"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="21330574"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="21330574"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Ops</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="12706079"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
@@ -841,16 +1210,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>755280</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>17280</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>18360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>683280</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>159840</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>728640</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>126360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -858,8 +1227,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7266960" y="9000"/>
-        <a:ext cx="7449120" cy="3402000"/>
+        <a:off x="1515240" y="1643760"/>
+        <a:ext cx="7396560" cy="4984920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -869,18 +1238,23 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>772560</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>27000</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>228960</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>36360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>29520</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>15120</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>139320</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>24840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -888,12 +1262,47 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7284240" y="3603240"/>
-        <a:ext cx="5942160" cy="3239280"/>
+        <a:off x="1726920" y="1011600"/>
+        <a:ext cx="5759640" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>134280</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>18000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>44280</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>6480</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="1787040" y="668160"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -968,10 +1377,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K36" activeCellId="0" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -981,25 +1390,25 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="B1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1026,6 +1435,10 @@
         <f aca="false">SUM(B2:F2)/5</f>
         <v>2720</v>
       </c>
+      <c r="H2" s="1" t="n">
+        <f aca="false">100 * 100 * 100 / G2</f>
+        <v>367.647058823529</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -1050,6 +1463,10 @@
         <f aca="false">SUM(B3:F3)/5</f>
         <v>1150</v>
       </c>
+      <c r="H3" s="1" t="n">
+        <f aca="false">100 * 100 * 100 / G3</f>
+        <v>869.565217391304</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -1074,6 +1491,10 @@
         <f aca="false">SUM(B4:F4)/5</f>
         <v>3130</v>
       </c>
+      <c r="H4" s="1" t="n">
+        <f aca="false">100 * 100 * 100 / G4</f>
+        <v>319.488817891374</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -1098,6 +1519,10 @@
         <f aca="false">SUM(B5:F5)/5</f>
         <v>942</v>
       </c>
+      <c r="H5" s="1" t="n">
+        <f aca="false">100 * 100 * 100 / G5</f>
+        <v>1061.57112526539</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -1122,6 +1547,10 @@
         <f aca="false">SUM(B6:F6)/5</f>
         <v>6600</v>
       </c>
+      <c r="H6" s="1" t="n">
+        <f aca="false">100 * 100 * 100 / G6</f>
+        <v>151.515151515152</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -1146,6 +1575,10 @@
         <f aca="false">SUM(B7:F7)/5</f>
         <v>1826</v>
       </c>
+      <c r="H7" s="1" t="n">
+        <f aca="false">100 * 100 * 100 / G7</f>
+        <v>547.645125958379</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -1170,100 +1603,253 @@
         <f aca="false">SUM(B8:F8)/5</f>
         <v>4078</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="H8" s="1" t="n">
+        <f aca="false">100 * 100 * 100 / G8</f>
+        <v>245.218244237371</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.8418367346939"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>2810</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>2770</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2820</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>2760</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>2910</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <f aca="false">SUM(B2:F2)/5</f>
+        <v>2814</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <f aca="false">100*100*50/G2</f>
+        <v>177.683013503909</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B3" s="0" t="n">
+        <v>27600</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>27030</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>27600</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>27180</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>27600</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">SUM(B3:F3)/5</f>
+        <v>27402</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <f aca="false">100*100*50/G3</f>
+        <v>18.2468432961098</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1630</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1630</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1640</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1530</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1630</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <f aca="false">SUM(B4:F4)/5</f>
+        <v>1612</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <f aca="false">100*100*50/G4</f>
+        <v>310.173697270471</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H44" activeCellId="0" sqref="H44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.8418367346939"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>10830</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>8050</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>11500</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>11310</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>11740</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <f aca="false">SUM(B2:F2)/5</f>
+        <v>10686</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <f aca="false">100*100*50/G2</f>
+        <v>46.7901927755942</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="0" t="n">
-        <v>4950</v>
-      </c>
-      <c r="C24" s="0" t="n">
-        <v>3080</v>
-      </c>
-      <c r="D24" s="0" t="n">
-        <v>4550</v>
-      </c>
-      <c r="E24" s="0" t="n">
-        <v>3740</v>
-      </c>
-      <c r="F24" s="0" t="n">
-        <v>3970</v>
-      </c>
-      <c r="G24" s="0" t="n">
-        <f aca="false">SUM(B24:F24)/5</f>
-        <v>4058</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="0" t="n">
-        <v>15200</v>
-      </c>
-      <c r="C25" s="0" t="n">
-        <v>11840</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>12690</v>
-      </c>
-      <c r="E25" s="0" t="n">
-        <v>12000</v>
-      </c>
-      <c r="F25" s="0" t="n">
-        <v>11950</v>
-      </c>
-      <c r="G25" s="0" t="n">
-        <f aca="false">SUM(B25:F25)/5</f>
-        <v>12736</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="0" t="n">
-        <v>2230</v>
-      </c>
-      <c r="C26" s="0" t="n">
-        <v>2080</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <v>2210</v>
-      </c>
-      <c r="E26" s="0" t="n">
-        <v>2080</v>
-      </c>
-      <c r="F26" s="0" t="n">
-        <v>2160</v>
-      </c>
-      <c r="G26" s="0" t="n">
-        <f aca="false">SUM(B26:F26)/5</f>
-        <v>2152</v>
+      <c r="B3" s="0" t="n">
+        <v>4720</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>4440</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>4610</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>4670</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>4670</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">SUM(B3:F3)/5</f>
+        <v>4622</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <f aca="false">100*100*50/G3</f>
+        <v>108.178277801817</v>
       </c>
     </row>
   </sheetData>

</xml_diff>